<commit_message>
s1-use filter table, check emty excel
</commit_message>
<xml_diff>
--- a/01_AutomationTest_Learn_V0.1/Utilities/Project1/Data_Project1.xlsx
+++ b/01_AutomationTest_Learn_V0.1/Utilities/Project1/Data_Project1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\02_MBS\01_PoC_AutomationTest\Test\Typical Testcase\UiPath\01_AutomationTest_Learn_V0.1\Utilities\Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14428428-8254-4715-AC6D-561FA33696CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF39875-85E5-4C90-8812-D7A16D63EE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="2505" windowWidth="16110" windowHeight="11400" xr2:uid="{041686C0-5BCB-4B5F-BBDD-DD4318C7E256}"/>
+    <workbookView xWindow="0" yWindow="2385" windowWidth="20265" windowHeight="11400" activeTab="1" xr2:uid="{041686C0-5BCB-4B5F-BBDD-DD4318C7E256}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Master" sheetId="1" r:id="rId1"/>
+    <sheet name="Work-Items2023" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,39 +37,135 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
   <si>
     <t>Type</t>
   </si>
   <si>
+    <t>Transaction</t>
+  </si>
+  <si>
     <t>Cash</t>
   </si>
   <si>
+    <t>WI1</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
     <t>WI2</t>
   </si>
   <si>
-    <t>WI1</t>
+    <t>W</t>
   </si>
   <si>
     <t>WI3</t>
   </si>
   <si>
+    <t>S</t>
+  </si>
+  <si>
     <t>WI4</t>
   </si>
   <si>
     <t>WI5</t>
   </si>
   <si>
-    <t>Transaction</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>S</t>
+    <t>WIID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>92928123</t>
+  </si>
+  <si>
+    <t>Verify Account Position</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>2023-05-25</t>
+  </si>
+  <si>
+    <t>92928061</t>
+  </si>
+  <si>
+    <t>Process Vendor Invoice</t>
+  </si>
+  <si>
+    <t>2023-01-19</t>
+  </si>
+  <si>
+    <t>92928134</t>
+  </si>
+  <si>
+    <t>2023-05-10</t>
+  </si>
+  <si>
+    <t>92928077</t>
+  </si>
+  <si>
+    <t>Research Client Check Copy</t>
+  </si>
+  <si>
+    <t>2023-04-03</t>
+  </si>
+  <si>
+    <t>92928072</t>
+  </si>
+  <si>
+    <t>2023-05-26</t>
+  </si>
+  <si>
+    <t>92928034</t>
+  </si>
+  <si>
+    <t>Calculate Client Security Hash</t>
+  </si>
+  <si>
+    <t>2023-01-08</t>
+  </si>
+  <si>
+    <t>92928127</t>
+  </si>
+  <si>
+    <t>2023-01-18</t>
+  </si>
+  <si>
+    <t>92928145</t>
+  </si>
+  <si>
+    <t>2023-04-27</t>
+  </si>
+  <si>
+    <t>92928068</t>
+  </si>
+  <si>
+    <t>92928024</t>
+  </si>
+  <si>
+    <t>2023-03-26</t>
+  </si>
+  <si>
+    <t>92928084</t>
+  </si>
+  <si>
+    <t>2023-02-12</t>
+  </si>
+  <si>
+    <t>92928064</t>
+  </si>
+  <si>
+    <t>2023-04-28</t>
   </si>
 </sst>
 </file>
@@ -435,12 +532,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423EC78C-1461-4EEE-B977-2E8E4F54F972}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -449,10 +547,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -460,7 +558,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -468,10 +566,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>200</v>
@@ -479,10 +577,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>300</v>
@@ -490,10 +588,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>1212</v>
@@ -501,10 +599,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>3232</v>
@@ -515,4 +613,243 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
 </file>
</xml_diff>